<commit_message>
feat: Nuevo dataset y estilos
</commit_message>
<xml_diff>
--- a/ResponseChatBot.xlsx
+++ b/ResponseChatBot.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="219">
   <si>
     <t>request</t>
   </si>
@@ -119,13 +119,562 @@
   </si>
   <si>
     <t>Solo debes decirme que necesitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bien </t>
+  </si>
+  <si>
+    <t>me alegro  ¿cuentame que necesitas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muy bien </t>
+  </si>
+  <si>
+    <t>todo bien</t>
+  </si>
+  <si>
+    <t>estoy bien</t>
+  </si>
+  <si>
+    <t>estoy vien</t>
+  </si>
+  <si>
+    <t>vien</t>
+  </si>
+  <si>
+    <t>perfecto</t>
+  </si>
+  <si>
+    <t>todo esta perfecto</t>
+  </si>
+  <si>
+    <t>me encuentro bien</t>
+  </si>
+  <si>
+    <t>me encuentro vien</t>
+  </si>
+  <si>
+    <t>¿quién eres?</t>
+  </si>
+  <si>
+    <t>¿qué haces?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿cómo te llamas? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿cómo estás? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿cómo funciona? </t>
+  </si>
+  <si>
+    <t>¿quien eres?</t>
+  </si>
+  <si>
+    <t>¿que haces?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿como te llamas? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿como estás? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿como funciona? </t>
+  </si>
+  <si>
+    <t>necesito ayuda</t>
+  </si>
+  <si>
+    <t>¿En que te ayudo?</t>
+  </si>
+  <si>
+    <t>ayudame en saber sobre</t>
+  </si>
+  <si>
+    <t>Te comunico con un asesor</t>
+  </si>
+  <si>
+    <t>q hubo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">que tal </t>
+  </si>
+  <si>
+    <t>como va</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> como lo trata la vida</t>
+  </si>
+  <si>
+    <t>bien ytu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saludo </t>
+  </si>
+  <si>
+    <t>Saludos</t>
+  </si>
+  <si>
+    <t>Q hubo</t>
+  </si>
+  <si>
+    <t>bieny tu</t>
+  </si>
+  <si>
+    <t>Quihubo</t>
+  </si>
+  <si>
+    <t>K tal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que tal </t>
+  </si>
+  <si>
+    <t>Como va</t>
+  </si>
+  <si>
+    <t>Bien y tu</t>
+  </si>
+  <si>
+    <t>Voy bien y tu</t>
+  </si>
+  <si>
+    <t>Yo estoy bien</t>
+  </si>
+  <si>
+    <t>Vien</t>
+  </si>
+  <si>
+    <t>Como lo trata la vida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenteme </t>
+  </si>
+  <si>
+    <t>Dime</t>
+  </si>
+  <si>
+    <t>dime</t>
+  </si>
+  <si>
+    <t>cuentame</t>
+  </si>
+  <si>
+    <t>Cuentame</t>
+  </si>
+  <si>
+    <t>Todo biencito</t>
+  </si>
+  <si>
+    <t>biencito</t>
+  </si>
+  <si>
+    <t>Biencito</t>
+  </si>
+  <si>
+    <t>Viencito</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bueno </t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bueno </t>
+  </si>
+  <si>
+    <t>Vueno</t>
+  </si>
+  <si>
+    <t>Muchas gracias</t>
+  </si>
+  <si>
+    <t>ten buen dia</t>
+  </si>
+  <si>
+    <t>Gracias</t>
+  </si>
+  <si>
+    <t>gracias</t>
+  </si>
+  <si>
+    <t>muchas gracias</t>
+  </si>
+  <si>
+    <t>Te agradezco</t>
+  </si>
+  <si>
+    <t>Cómo estas</t>
+  </si>
+  <si>
+    <t>¿Cómo estás?</t>
+  </si>
+  <si>
+    <t>¿Cuentame tu día ?</t>
+  </si>
+  <si>
+    <t>Como estás?</t>
+  </si>
+  <si>
+    <t>Como estas</t>
+  </si>
+  <si>
+    <t>El dia estuvo bien</t>
+  </si>
+  <si>
+    <t>El día estuvo bien</t>
+  </si>
+  <si>
+    <t>El dia estubo bien</t>
+  </si>
+  <si>
+    <t>El dia estuvo vien</t>
+  </si>
+  <si>
+    <t>el dia estuvo bien</t>
+  </si>
+  <si>
+    <t>el día estuvo bien</t>
+  </si>
+  <si>
+    <t>el dia estubo bien</t>
+  </si>
+  <si>
+    <t>el dia estuvo vien</t>
+  </si>
+  <si>
+    <t>Holita</t>
+  </si>
+  <si>
+    <t>olita</t>
+  </si>
+  <si>
+    <t>Olita</t>
+  </si>
+  <si>
+    <t>vuenas</t>
+  </si>
+  <si>
+    <t>vuenas tardes</t>
+  </si>
+  <si>
+    <t>vuenas noches</t>
+  </si>
+  <si>
+    <t>vuenos dias</t>
+  </si>
+  <si>
+    <t>Buenas</t>
+  </si>
+  <si>
+    <t>Buenas tardes</t>
+  </si>
+  <si>
+    <t>Buenas noches</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>Ey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adios </t>
+  </si>
+  <si>
+    <t>Vuelve pronto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chao </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasta luego </t>
+  </si>
+  <si>
+    <t>oki</t>
+  </si>
+  <si>
+    <t>helo</t>
+  </si>
+  <si>
+    <t>jelo</t>
+  </si>
+  <si>
+    <t>bot</t>
+  </si>
+  <si>
+    <t>bot que tal</t>
+  </si>
+  <si>
+    <t>regresé</t>
+  </si>
+  <si>
+    <t>bot como estas</t>
+  </si>
+  <si>
+    <t>como te sientes</t>
+  </si>
+  <si>
+    <t>bot como vas</t>
+  </si>
+  <si>
+    <t>bot hola</t>
+  </si>
+  <si>
+    <t>botsito</t>
+  </si>
+  <si>
+    <t>Bot</t>
+  </si>
+  <si>
+    <t>bot como vai</t>
+  </si>
+  <si>
+    <t>bot como has estado</t>
+  </si>
+  <si>
+    <t>bot como te ha ido</t>
+  </si>
+  <si>
+    <t>bot como va todo</t>
+  </si>
+  <si>
+    <t>bot como te va</t>
+  </si>
+  <si>
+    <t>bot, buenas noches</t>
+  </si>
+  <si>
+    <t>bot, buenas tardes</t>
+  </si>
+  <si>
+    <t>suerte bot!!!</t>
+  </si>
+  <si>
+    <t>ADIOS</t>
+  </si>
+  <si>
+    <t>adios bot</t>
+  </si>
+  <si>
+    <t>ah que bien, hasta luego</t>
+  </si>
+  <si>
+    <t>ah, adios</t>
+  </si>
+  <si>
+    <t>aja, chaolin</t>
+  </si>
+  <si>
+    <t>bye bye#$</t>
+  </si>
+  <si>
+    <t>bye bot</t>
+  </si>
+  <si>
+    <t>cancelar</t>
+  </si>
+  <si>
+    <t>cancelar proceso</t>
+  </si>
+  <si>
+    <t>capito, chau</t>
+  </si>
+  <si>
+    <t>chao</t>
+  </si>
+  <si>
+    <t>chaolin</t>
+  </si>
+  <si>
+    <t>chau</t>
+  </si>
+  <si>
+    <t>chao bot</t>
+  </si>
+  <si>
+    <t>nos vemos</t>
+  </si>
+  <si>
+    <t>chau, hablamos</t>
+  </si>
+  <si>
+    <t>chauuu GRacias!!!</t>
+  </si>
+  <si>
+    <t>quiero salirme de esto</t>
+  </si>
+  <si>
+    <t>cancelar esta conversación</t>
+  </si>
+  <si>
+    <t>dale, chau</t>
+  </si>
+  <si>
+    <t>debo irme, chaolin</t>
+  </si>
+  <si>
+    <t>entendí, chaolin</t>
+  </si>
+  <si>
+    <t>entendido, chau</t>
+  </si>
+  <si>
+    <t>eres muy amable bot, adios</t>
+  </si>
+  <si>
+    <t>no quiero seguir, cancelar</t>
+  </si>
+  <si>
+    <t>esta bien, chau</t>
+  </si>
+  <si>
+    <t>gracias por todo, adios,</t>
+  </si>
+  <si>
+    <t>gracias sofi</t>
+  </si>
+  <si>
+    <t>oki doki, adios</t>
+  </si>
+  <si>
+    <t>todo bien, bot</t>
+  </si>
+  <si>
+    <t>gracias, hasta luego</t>
+  </si>
+  <si>
+    <t>hasta luego</t>
+  </si>
+  <si>
+    <t>hasta luego bot</t>
+  </si>
+  <si>
+    <t>hasta pronto!!</t>
+  </si>
+  <si>
+    <t>igual chao</t>
+  </si>
+  <si>
+    <t>listo, hasta luego</t>
+  </si>
+  <si>
+    <t>me quiero salir de esta conversación</t>
+  </si>
+  <si>
+    <t>ok, chau</t>
+  </si>
+  <si>
+    <t>muchas gracias, adios</t>
+  </si>
+  <si>
+    <t>no me sirvió la info, adios</t>
+  </si>
+  <si>
+    <t>no quiero hablar mas</t>
+  </si>
+  <si>
+    <t>no deseo hablar, cancelar</t>
+  </si>
+  <si>
+    <t>no quiero nada</t>
+  </si>
+  <si>
+    <t>no quiero seguir</t>
+  </si>
+  <si>
+    <t>no quiero seguir en este proceso</t>
+  </si>
+  <si>
+    <t>no quiero seguir, voy a salir</t>
+  </si>
+  <si>
+    <t>nos vemos sofi</t>
+  </si>
+  <si>
+    <t>nos vemos robotina</t>
+  </si>
+  <si>
+    <t>ok bye</t>
+  </si>
+  <si>
+    <t>ok, suerte</t>
+  </si>
+  <si>
+    <t>ok bye sofy</t>
+  </si>
+  <si>
+    <t>ok, feliz día</t>
+  </si>
+  <si>
+    <t>oki doki, chau</t>
+  </si>
+  <si>
+    <t>oka, bye</t>
+  </si>
+  <si>
+    <t>bot, cancela esta conversación</t>
+  </si>
+  <si>
+    <t>no me sirve, cancela mi peticion</t>
+  </si>
+  <si>
+    <t>que estés bien</t>
+  </si>
+  <si>
+    <t>no seguir con esto</t>
+  </si>
+  <si>
+    <t>que tengas un feliz dia</t>
+  </si>
+  <si>
+    <t>cancela mi solicitud</t>
+  </si>
+  <si>
+    <t>salgo de esta conversación</t>
+  </si>
+  <si>
+    <t>salir</t>
+  </si>
+  <si>
+    <t>salir de la conversación</t>
+  </si>
+  <si>
+    <t>see you</t>
+  </si>
+  <si>
+    <t>siclas, chaolin</t>
+  </si>
+  <si>
+    <t>sisas, suerte</t>
+  </si>
+  <si>
+    <t>cancela este proceso</t>
+  </si>
+  <si>
+    <t>cancelar todo</t>
+  </si>
+  <si>
+    <t>no quiero seguir con esto</t>
+  </si>
+  <si>
+    <t>suerte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -136,6 +685,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,12 +706,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,6 +933,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
+    <col customWidth="1" min="2" max="2" width="26.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -578,6 +1136,1478 @@
         <v>35</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Cambios en dataset
</commit_message>
<xml_diff>
--- a/ResponseChatBot.xlsx
+++ b/ResponseChatBot.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="219">
   <si>
     <t>request</t>
   </si>
@@ -112,9 +112,6 @@
     <t xml:space="preserve">Hola soy bot </t>
   </si>
   <si>
-    <t xml:space="preserve">¿Cómo estás? </t>
-  </si>
-  <si>
     <t xml:space="preserve">¿Cómo funciona? </t>
   </si>
   <si>
@@ -229,12 +226,6 @@
     <t>K tal</t>
   </si>
   <si>
-    <t xml:space="preserve">Que tal </t>
-  </si>
-  <si>
-    <t>Como va</t>
-  </si>
-  <si>
     <t>Bien y tu</t>
   </si>
   <si>
@@ -250,21 +241,18 @@
     <t>Como lo trata la vida</t>
   </si>
   <si>
+    <t>Dime</t>
+  </si>
+  <si>
+    <t>dime</t>
+  </si>
+  <si>
+    <t>cuentame</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cuenteme </t>
   </si>
   <si>
-    <t>Dime</t>
-  </si>
-  <si>
-    <t>dime</t>
-  </si>
-  <si>
-    <t>cuentame</t>
-  </si>
-  <si>
-    <t>Cuentame</t>
-  </si>
-  <si>
     <t>Todo biencito</t>
   </si>
   <si>
@@ -310,24 +298,6 @@
     <t>Te agradezco</t>
   </si>
   <si>
-    <t>Cómo estas</t>
-  </si>
-  <si>
-    <t>¿Cómo estás?</t>
-  </si>
-  <si>
-    <t>¿Cuentame tu día ?</t>
-  </si>
-  <si>
-    <t>Como estás?</t>
-  </si>
-  <si>
-    <t>Como estas</t>
-  </si>
-  <si>
-    <t>El dia estuvo bien</t>
-  </si>
-  <si>
     <t>El día estuvo bien</t>
   </si>
   <si>
@@ -337,18 +307,6 @@
     <t>El dia estuvo vien</t>
   </si>
   <si>
-    <t>el dia estuvo bien</t>
-  </si>
-  <si>
-    <t>el día estuvo bien</t>
-  </si>
-  <si>
-    <t>el dia estubo bien</t>
-  </si>
-  <si>
-    <t>el dia estuvo vien</t>
-  </si>
-  <si>
     <t>Holita</t>
   </si>
   <si>
@@ -439,6 +397,9 @@
     <t>bot como vai</t>
   </si>
   <si>
+    <t>no entiendo la pregunta</t>
+  </si>
+  <si>
     <t>bot como has estado</t>
   </si>
   <si>
@@ -460,6 +421,9 @@
     <t>suerte bot!!!</t>
   </si>
   <si>
+    <t>Ten un buen día</t>
+  </si>
+  <si>
     <t>ADIOS</t>
   </si>
   <si>
@@ -475,7 +439,7 @@
     <t>aja, chaolin</t>
   </si>
   <si>
-    <t>bye bye#$</t>
+    <t>bye bye</t>
   </si>
   <si>
     <t>bye bot</t>
@@ -652,7 +616,7 @@
     <t>see you</t>
   </si>
   <si>
-    <t>siclas, chaolin</t>
+    <t>sisas, chaolin</t>
   </si>
   <si>
     <t>sisas, suerte</t>
@@ -668,6 +632,42 @@
   </si>
   <si>
     <t>suerte</t>
+  </si>
+  <si>
+    <t>color favorito</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>sds</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>fdfgghfdgfdgdg</t>
+  </si>
+  <si>
+    <t>altura</t>
+  </si>
+  <si>
+    <t>que</t>
+  </si>
+  <si>
+    <t>como</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>como asi</t>
   </si>
 </sst>
 </file>
@@ -932,7 +932,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.25"/>
+    <col customWidth="1" min="1" max="1" width="39.5"/>
     <col customWidth="1" min="2" max="2" width="26.63"/>
   </cols>
   <sheetData>
@@ -1125,23 +1125,23 @@
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="27">
@@ -1149,7 +1149,7 @@
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
@@ -1157,7 +1157,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
@@ -1165,7 +1165,7 @@
         <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
@@ -1173,7 +1173,7 @@
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
@@ -1181,7 +1181,7 @@
         <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
@@ -1189,7 +1189,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
@@ -1197,7 +1197,7 @@
         <v>44</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
@@ -1205,7 +1205,7 @@
         <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
@@ -1213,7 +1213,7 @@
         <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
@@ -1221,7 +1221,7 @@
         <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37">
@@ -1229,7 +1229,7 @@
         <v>48</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
@@ -1237,7 +1237,7 @@
         <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
@@ -1245,7 +1245,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40">
@@ -1253,7 +1253,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41">
@@ -1261,7 +1261,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42">
@@ -1269,7 +1269,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43">
@@ -1277,7 +1277,7 @@
         <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
@@ -1285,7 +1285,7 @@
         <v>55</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45">
@@ -1293,23 +1293,23 @@
         <v>56</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48">
@@ -1317,7 +1317,7 @@
         <v>61</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49">
@@ -1333,15 +1333,15 @@
         <v>63</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52">
@@ -1357,15 +1357,15 @@
         <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55">
@@ -1389,7 +1389,7 @@
         <v>72</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
@@ -1397,7 +1397,7 @@
         <v>73</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
@@ -1405,7 +1405,7 @@
         <v>74</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60">
@@ -1413,7 +1413,7 @@
         <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61">
@@ -1421,7 +1421,7 @@
         <v>76</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62">
@@ -1429,7 +1429,7 @@
         <v>77</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63">
@@ -1437,7 +1437,7 @@
         <v>78</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64">
@@ -1445,7 +1445,7 @@
         <v>79</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65">
@@ -1453,7 +1453,7 @@
         <v>80</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
@@ -1461,7 +1461,7 @@
         <v>81</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67">
@@ -1469,268 +1469,268 @@
         <v>82</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>28</v>
@@ -1738,143 +1738,143 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="s">
-        <v>115</v>
+      <c r="A102" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="s">
-        <v>116</v>
+      <c r="A103" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="s">
-        <v>117</v>
+      <c r="A104" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="s">
-        <v>118</v>
+      <c r="A105" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="s">
-        <v>119</v>
+      <c r="A106" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="s">
-        <v>120</v>
+      <c r="A107" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="s">
-        <v>121</v>
+      <c r="A108" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="s">
-        <v>9</v>
+      <c r="A109" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="s">
-        <v>122</v>
+      <c r="A110" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="s">
-        <v>123</v>
+      <c r="A111" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="B116" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="s">
-        <v>130</v>
+      <c r="A117" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="s">
-        <v>131</v>
+      <c r="A118" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>28</v>
@@ -1882,730 +1882,706 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="s">
-        <v>138</v>
+        <v>26</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="2" t="s">
-        <v>202</v>
+      <c r="A193" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="2" t="s">
-        <v>203</v>
+      <c r="A194" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="2" t="s">
-        <v>204</v>
+      <c r="A195" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="2" t="s">
-        <v>205</v>
+      <c r="A196" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="2" t="s">
-        <v>206</v>
+      <c r="A197" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="2" t="s">
-        <v>207</v>
+      <c r="A198" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="2" t="s">
-        <v>208</v>
+      <c r="A199" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="2" t="s">
-        <v>209</v>
+      <c r="A200" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="2" t="s">
-        <v>210</v>
+      <c r="A201" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="2" t="s">
-        <v>211</v>
+      <c r="A202" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="2" t="s">
-        <v>212</v>
+      <c r="A203" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="2" t="s">
-        <v>213</v>
+      <c r="A204" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="2" t="s">
-        <v>214</v>
+      <c r="A205" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="2" t="s">
-        <v>215</v>
+      <c r="A206" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>